<commit_message>
Afni budget approval test
</commit_message>
<xml_diff>
--- a/RR/excel/NominationFlow/Nomination.xlsx
+++ b/RR/excel/NominationFlow/Nomination.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AC\git\RR_Web_Automation\RR\excel\NominationFlow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81824EB8-7B6B-494B-AF3A-E521416F443E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC9D24D-6684-426C-B1E4-4DA4DA15ADA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C37C6F66-C3C9-4B21-8A13-A93D29D3A7D2}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
   <si>
     <t>Appriciate Details</t>
   </si>
@@ -237,12 +237,19 @@
   </si>
   <si>
     <t xml:space="preserve">Award no. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Budget requester flow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -687,20 +694,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5535AA-3ED3-41CB-8E9C-ECDE303779DB}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="31.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="34.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" style="4" width="29.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="33.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="31.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.21875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="34.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -846,6 +853,9 @@
       <c r="A17" s="14" t="s">
         <v>52</v>
       </c>
+      <c r="B17" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D18" s="4"/>
@@ -881,6 +891,14 @@
       <c r="B21" s="3"/>
       <c r="D21" s="4"/>
       <c r="E21" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1014.0</v>
+      </c>
     </row>
     <row r="24" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">

</xml_diff>